<commit_message>
Added More test cases for Updating, Creating, and Reading KPIs and Assessments
</commit_message>
<xml_diff>
--- a/TestCases/Back End/CreateAssessment-BackEnd-ServiceManager.xlsx
+++ b/TestCases/Back End/CreateAssessment-BackEnd-ServiceManager.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18801"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{C4752288-1FFB-4E83-9E5F-4F7975B6A37C}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{D024CBF3-B622-40E7-8894-04E62C3F604E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{C4752288-1FFB-4E83-9E5F-4F7975B6A37C}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{D024CBF3-B622-40E7-8894-04E62C3F604E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>